<commit_message>
Added stuff like pictures, pdf doc etc.
</commit_message>
<xml_diff>
--- a/Assignment1/excel/Charts.xlsx
+++ b/Assignment1/excel/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timur\OneDrive\Desktop\CS\3. Semester\Human-Computer Interaction\HCI\Assignment1\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE0CEE19-1D15-45CE-83CC-124E70D66F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E216046D-8AF3-421F-A2D4-39ACB88DD4A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD31C7D9-813E-4ED4-8F83-428347D8E7F9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Participant</t>
   </si>
@@ -44,10 +44,22 @@
     <t>SD</t>
   </si>
   <si>
-    <t>Ahmet</t>
+    <t>P1</t>
   </si>
   <si>
-    <t>Berat</t>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
   </si>
 </sst>
 </file>
@@ -132,11 +144,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -145,8 +156,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-DK"/>
-              <a:t>Trial 1</a:t>
+              <a:rPr lang="da-DK"/>
+              <a:t>Average Reaction Times and Its Deviation</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -164,11 +175,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -190,16 +200,91 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
@@ -211,7 +296,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>162</c:v>
+                    <c:v>184</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -223,18 +308,17 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>162</c:v>
+                    <c:v>184</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
@@ -249,30 +333,105 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>608</c:v>
+                  <c:v>668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F616-4FB7-9C99-52F2A000D37F}"/>
+              <c16:uniqueId val="{00000000-B1D1-428C-869B-9E5727FB4B3A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
@@ -284,7 +443,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>112</c:v>
+                    <c:v>119</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -296,18 +455,17 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>112</c:v>
+                    <c:v>119</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
@@ -322,75 +480,656 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>528</c:v>
+                  <c:v>574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F616-4FB7-9C99-52F2A000D37F}"/>
+              <c16:uniqueId val="{00000001-B1D1-428C-869B-9E5727FB4B3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$D$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$D$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B1D1-428C-869B-9E5727FB4B3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>235</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>235</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>581</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B1D1-428C-869B-9E5727FB4B3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>132</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$F$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>132</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>450</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B1D1-428C-869B-9E5727FB4B3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent6">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$G$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>108</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>108</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>418</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B1D1-428C-869B-9E5727FB4B3A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1598367455"/>
-        <c:axId val="1518089007"/>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
+        <c:axId val="129052048"/>
+        <c:axId val="135231904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1598367455"/>
+        <c:axId val="129052048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1518089007"/>
+        <c:crossAx val="135231904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -398,7 +1137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1518089007"/>
+        <c:axId val="135231904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,12 +1146,23 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -436,9 +1186,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -449,7 +1198,7 @@
             <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1598367455"/>
+        <c:crossAx val="129052048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -462,7 +1211,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -478,9 +1227,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -498,11 +1246,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -524,7 +1275,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -570,33 +1321,46 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -605,38 +1369,14 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -646,23 +1386,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -670,71 +1405,131 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:effectRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -750,26 +1545,47 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
+  </cs:downBar>
+  <cs:dropLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -777,35 +1593,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -817,14 +1608,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -836,30 +1626,35 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -869,16 +1664,29 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -888,14 +1696,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -907,14 +1714,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -926,27 +1732,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -954,9 +1759,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -966,14 +1770,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -985,12 +1788,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -999,14 +1801,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1015,9 +1818,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1031,15 +1833,17 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1048,9 +1852,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1060,14 +1863,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1076,23 +1873,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4338B88C-48F8-422A-BCA0-A3D953C7810B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCF3BD3-DFD8-4218-BCFE-9CE1C0E34A71}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1410,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6076A0BB-C369-49C0-9399-7428B11458E8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,7 +2221,7 @@
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1434,27 +2231,63 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>608</v>
+        <v>668</v>
       </c>
       <c r="C2" s="1">
-        <v>528</v>
+        <v>574</v>
+      </c>
+      <c r="D2">
+        <v>665</v>
+      </c>
+      <c r="E2">
+        <v>581</v>
+      </c>
+      <c r="F2">
+        <v>450</v>
+      </c>
+      <c r="G2">
+        <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="C3" s="1">
-        <v>112</v>
+        <v>119</v>
+      </c>
+      <c r="D3">
+        <v>203</v>
+      </c>
+      <c r="E3">
+        <v>235</v>
+      </c>
+      <c r="F3">
+        <v>132</v>
+      </c>
+      <c r="G3">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>